<commit_message>
Simulation n'arrête plus pour valeurs hors limite et placettes non simulées ajoutées au fichier des simulations
</commit_message>
<xml_diff>
--- a/data-raw/Validation_intrants.xlsx
+++ b/data-raw/Validation_intrants.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projets\IsabelleAuger\Natura\RNatura2014\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Projets\IsabelleAuger\Natura\Natura2014\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806EC7B1-B990-4E62-91A2-EF40B68BEB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F59850-4857-4E51-A3D6-09A7F5F68A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34BCFCC6-80BC-476A-BD53-DAC99D297AB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{34BCFCC6-80BC-476A-BD53-DAC99D297AB0}"/>
   </bookViews>
   <sheets>
     <sheet name="valid" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">valid!$D$1:$D$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">valid!$D$1:$D$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
   <si>
     <t>essence</t>
   </si>
@@ -56,9 +56,6 @@
     <t>dhpcm</t>
   </si>
   <si>
-    <t>etat</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>vft &lt; 500</t>
   </si>
   <si>
-    <t>etat %in% c('10', '12', '40', '42', '30', '32', '50', '52')</t>
-  </si>
-  <si>
     <t>substr(type_eco,1,3) %in% vp_retenues</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
   </si>
   <si>
     <t>Code d'essence a l'exterieur de la plage de valeurs possibles</t>
-  </si>
-  <si>
-    <t>Code d'etat a l'exterieur de la plage de valeurs possibles (10, 12, 30, 32, 40, 42, 50, 52)</t>
   </si>
   <si>
     <t>Latitude a l'exterieur de la plage de valeurs possibles (44.9 et &lt; 52.5)</t>
@@ -430,12 +421,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -461,9 +451,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -501,7 +491,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -607,7 +597,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -749,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -757,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,232 +761,217 @@
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>70</v>
+        <v>108</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>112</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1004,10 +979,10 @@
         <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1015,13 +990,13 @@
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,10 +1007,10 @@
         <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,38 +1021,38 @@
         <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1085,13 +1060,13 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,13 +1074,13 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,38 +1091,38 @@
         <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,10 +1133,10 @@
         <v>63</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,13 +1144,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,55 +1158,55 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,13 +1214,13 @@
         <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,31 +1228,17 @@
         <v>35</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D35" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}"/>
+  <autoFilter ref="D1:D34" xr:uid="{E5AF6700-1036-4ACC-BE6D-6C464A378F49}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>